<commit_message>
db changes to both frontend and backend
</commit_message>
<xml_diff>
--- a/db/account_weekly_snapshot.xlsx
+++ b/db/account_weekly_snapshot.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,7 +812,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Crypto</t>
+          <t>Coinbase</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -821,30 +821,26 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>783.76</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2025-06-20</t>
-        </is>
+        <v>36510.98</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" s="2" t="n">
+        <v>45830.15939476852</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>401K</t>
+          <t>Crypto</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> stocks</t>
+          <t xml:space="preserve"> crypto</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>25004.86</v>
+        <v>783.76</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -858,7 +854,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>401kM</t>
+          <t>401K</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -867,7 +863,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2922.05</v>
+        <v>25004.86</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -881,7 +877,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CGI</t>
+          <t>401kM</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -890,7 +886,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8276.860000000001</v>
+        <v>2922.05</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -904,7 +900,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HSA</t>
+          <t>CGI</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -913,7 +909,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5738.01</v>
+        <v>8276.860000000001</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -927,7 +923,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Robinhood</t>
+          <t>HSA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -936,7 +932,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7098.08</v>
+        <v>5738.01</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -950,7 +946,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RobinhoodM</t>
+          <t>Robinhood</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -959,7 +955,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>9383.99</v>
+        <v>7098.08</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -973,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Schwab</t>
+          <t>RobinhoodM</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -982,7 +978,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9494.98</v>
+        <v>9383.99</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -996,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Webull</t>
+          <t>RobinhoodM</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1005,36 +1001,78 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>16</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2025-06-20</t>
-        </is>
+        <v>8824.620000000001</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" s="2" t="n">
+        <v>45830.16335171296</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Coinbase</t>
+          <t>Schwab</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t xml:space="preserve"> stocks</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>9494.98</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2025-06-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Webull</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> stocks</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>16</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2025-06-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Crypto</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t xml:space="preserve"> crypto</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>36595.08</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" s="2" t="n">
-        <v>45830</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>732.41</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" s="2" t="n">
+        <v>45830.16999824475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>